<commit_message>
fix(working-calendar): crud working calendar
</commit_message>
<xml_diff>
--- a/public/working_calendar_data.xlsx
+++ b/public/working_calendar_data.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -413,21 +413,90 @@
         <v>date</v>
       </c>
       <c r="D1" t="str">
-        <v>start</v>
+        <v>type</v>
       </c>
       <c r="E1" t="str">
-        <v>end</v>
+        <v>description</v>
       </c>
       <c r="F1" t="str">
-        <v>type</v>
+        <v/>
       </c>
       <c r="G1" t="str">
-        <v>description</v>
+        <v/>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>C001</v>
+      </c>
+      <c r="B2" t="str">
+        <v>B001</v>
+      </c>
+      <c r="C2" t="str">
+        <v>2024-01-01</v>
+      </c>
+      <c r="D2" t="str">
+        <v>working day</v>
+      </c>
+      <c r="E2" t="str">
+        <v>hari kerja</v>
+      </c>
+      <c r="F2" t="str">
+        <v/>
+      </c>
+      <c r="G2" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>C001</v>
+      </c>
+      <c r="B3" t="str">
+        <v>B001</v>
+      </c>
+      <c r="C3" t="str">
+        <v>2024-01-02</v>
+      </c>
+      <c r="D3" t="str">
+        <v>event</v>
+      </c>
+      <c r="E3" t="str">
+        <v>event</v>
+      </c>
+      <c r="F3" t="str">
+        <v/>
+      </c>
+      <c r="G3" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>C001</v>
+      </c>
+      <c r="B4" t="str">
+        <v>B001</v>
+      </c>
+      <c r="C4" t="str">
+        <v>2024-01-03</v>
+      </c>
+      <c r="D4" t="str">
+        <v>holiday</v>
+      </c>
+      <c r="E4" t="str">
+        <v>libur</v>
+      </c>
+      <c r="F4" t="str">
+        <v/>
+      </c>
+      <c r="G4" t="str">
+        <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix(department): make edit works and create department import with standalone component
</commit_message>
<xml_diff>
--- a/public/working_calendar_data.xlsx
+++ b/public/working_calendar_data.xlsx
@@ -397,14 +397,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>comp_code</v>
+        <v>company_code</v>
       </c>
       <c r="B1" t="str">
         <v>branch_code</v>
@@ -417,12 +417,6 @@
       </c>
       <c r="E1" t="str">
         <v>description</v>
-      </c>
-      <c r="F1" t="str">
-        <v/>
-      </c>
-      <c r="G1" t="str">
-        <v/>
       </c>
     </row>
     <row r="2">
@@ -433,19 +427,13 @@
         <v>B001</v>
       </c>
       <c r="C2" t="str">
-        <v>2024-01-01</v>
+        <v>2024-10-21</v>
       </c>
       <c r="D2" t="str">
         <v>working day</v>
       </c>
       <c r="E2" t="str">
         <v>hari kerja</v>
-      </c>
-      <c r="F2" t="str">
-        <v/>
-      </c>
-      <c r="G2" t="str">
-        <v/>
       </c>
     </row>
     <row r="3">
@@ -453,50 +441,21 @@
         <v>C001</v>
       </c>
       <c r="B3" t="str">
-        <v>B001</v>
+        <v>B002</v>
       </c>
       <c r="C3" t="str">
-        <v>2024-01-02</v>
+        <v>2024-10-22</v>
       </c>
       <c r="D3" t="str">
-        <v>event</v>
+        <v>holiday</v>
       </c>
       <c r="E3" t="str">
-        <v>event</v>
-      </c>
-      <c r="F3" t="str">
-        <v/>
-      </c>
-      <c r="G3" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>C001</v>
-      </c>
-      <c r="B4" t="str">
-        <v>B001</v>
-      </c>
-      <c r="C4" t="str">
-        <v>2024-01-03</v>
-      </c>
-      <c r="D4" t="str">
-        <v>holiday</v>
-      </c>
-      <c r="E4" t="str">
-        <v>libur</v>
-      </c>
-      <c r="F4" t="str">
-        <v/>
-      </c>
-      <c r="G4" t="str">
-        <v/>
+        <v>hari libu</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>